<commit_message>
UPD: Add detection if not free parking position and get car on detect out rectangle
</commit_message>
<xml_diff>
--- a/Telegram/Data/users.xlsx
+++ b/Telegram/Data/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="426">
   <si>
     <t>Telegram ID</t>
   </si>
@@ -40,162 +40,162 @@
     <t>Миннебаева Аделина Ильнуровна</t>
   </si>
   <si>
+    <t>Зиганшин Камиль Айратович</t>
+  </si>
+  <si>
+    <t>Валиахметов Динар Русланович</t>
+  </si>
+  <si>
+    <t>Валова Юлия Анатольевна</t>
+  </si>
+  <si>
+    <t>Садыков Тимур Русланович</t>
+  </si>
+  <si>
+    <t>Хуснутдинов Эльдар Александрович</t>
+  </si>
+  <si>
+    <t>Сабирзянов Риаз Римович</t>
+  </si>
+  <si>
+    <t>Вахитов Камиль Рамилович</t>
+  </si>
+  <si>
+    <t>Потапова Елена Владимировна</t>
+  </si>
+  <si>
+    <t>Кондратьев Данила Андреевич</t>
+  </si>
+  <si>
+    <t>Горячев Никита Евгеньевич</t>
+  </si>
+  <si>
+    <t>Абзалов Ильяс Радикович</t>
+  </si>
+  <si>
+    <t>Хайдаров Ильяс Ильшатоаич</t>
+  </si>
+  <si>
+    <t>Фаттахова Камилла Амировна</t>
+  </si>
+  <si>
+    <t>Аникович Владислав Витальевич</t>
+  </si>
+  <si>
+    <t>Досеев Илья Алексеевич</t>
+  </si>
+  <si>
+    <t>Тютюгин Кирилл Денисович</t>
+  </si>
+  <si>
+    <t>Чумаков Алексей Вадимович</t>
+  </si>
+  <si>
+    <t>Шугулева Елена Сергеевна</t>
+  </si>
+  <si>
+    <t>Калякин Владислав Викторович</t>
+  </si>
+  <si>
+    <t>Хабибуллин Азат Фаритович</t>
+  </si>
+  <si>
+    <t>Шамсуллина Элина Рустемовна</t>
+  </si>
+  <si>
+    <t>Галиев Камиль Айратович</t>
+  </si>
+  <si>
+    <t>Шамсиев Эльдар Халилович</t>
+  </si>
+  <si>
+    <t>Гайнуллин Ильнур Ильхамович</t>
+  </si>
+  <si>
+    <t>Чукашов Вячеслав Николаевич</t>
+  </si>
+  <si>
+    <t>Махмутов Амир Фаридович</t>
+  </si>
+  <si>
+    <t>Лисицких Вероника Валериановна</t>
+  </si>
+  <si>
+    <t>Шайдуллин Никита Рустемович</t>
+  </si>
+  <si>
+    <t>Ахметзянов Ренат Ибрагимович</t>
+  </si>
+  <si>
+    <t>Соколова Юлия Алексеевна</t>
+  </si>
+  <si>
+    <t>Ларионов Алексей Андреевич</t>
+  </si>
+  <si>
+    <t>Петряев Вадим Витальевич</t>
+  </si>
+  <si>
+    <t>Пискунов Дмитрий Андреевич</t>
+  </si>
+  <si>
+    <t>Бауличева Кристина Викторовна</t>
+  </si>
+  <si>
+    <t>Хабирзянова Ралина Разиловна</t>
+  </si>
+  <si>
+    <t>Галимзянов Руслан Рефатович</t>
+  </si>
+  <si>
+    <t>Шамсутдинов Ранис Рамилевич</t>
+  </si>
+  <si>
+    <t>Ханипова Регина Рамилевна</t>
+  </si>
+  <si>
+    <t>Замалеева Гузель Ринатовна</t>
+  </si>
+  <si>
+    <t>Гайфуллин Илдус Миннахматович</t>
+  </si>
+  <si>
+    <t>Мисбахов Рустам Шаукатович</t>
+  </si>
+  <si>
+    <t>Салихов Ильнар Рамилевич</t>
+  </si>
+  <si>
+    <t>Емельянов Дмитрий Владимирович</t>
+  </si>
+  <si>
+    <t>Мокшин Владимир Васильевич</t>
+  </si>
+  <si>
+    <t>Сайфудинов Ильдар Рифатович</t>
+  </si>
+  <si>
+    <t>Сарачева Диана Азатовна</t>
+  </si>
+  <si>
+    <t>Шипилова Ольга Александровна</t>
+  </si>
+  <si>
+    <t>Хасаншина Эльвира Маратовна</t>
+  </si>
+  <si>
+    <t>Минкин Марат Риналович</t>
+  </si>
+  <si>
+    <t>Ильин Алексей Николаевич</t>
+  </si>
+  <si>
+    <t>Ахметзянов Айнур Фагилевич</t>
+  </si>
+  <si>
     <t>Рамазанов Ришат Рафаэлевич</t>
   </si>
   <si>
-    <t>Зиганшин Камиль Айратович</t>
-  </si>
-  <si>
-    <t>Валиахметов Динар Русланович</t>
-  </si>
-  <si>
-    <t>Валова Юлия Анатольевна</t>
-  </si>
-  <si>
-    <t>Садыков Тимур Русланович</t>
-  </si>
-  <si>
-    <t>Хуснутдинов Эльдар Александрович</t>
-  </si>
-  <si>
-    <t>Сабирзянов Риаз Римович</t>
-  </si>
-  <si>
-    <t>Вахитов Камиль Рамилович</t>
-  </si>
-  <si>
-    <t>Потапова Елена Владимировна</t>
-  </si>
-  <si>
-    <t>Кондратьев Данила Андреевич</t>
-  </si>
-  <si>
-    <t>Горячев Никита Евгеньевич</t>
-  </si>
-  <si>
-    <t>Абзалов Ильяс Радикович</t>
-  </si>
-  <si>
-    <t>Хайдаров Ильяс Ильшатоаич</t>
-  </si>
-  <si>
-    <t>Фаттахова Камилла Амировна</t>
-  </si>
-  <si>
-    <t>Аникович Владислав Витальевич</t>
-  </si>
-  <si>
-    <t>Досеев Илья Алексеевич</t>
-  </si>
-  <si>
-    <t>Тютюгин Кирилл Денисович</t>
-  </si>
-  <si>
-    <t>Чумаков Алексей Вадимович</t>
-  </si>
-  <si>
-    <t>Шугулева Елена Сергеевна</t>
-  </si>
-  <si>
-    <t>Калякин Владислав Викторович</t>
-  </si>
-  <si>
-    <t>Хабибуллин Азат Фаритович</t>
-  </si>
-  <si>
-    <t>Шамсуллина Элина Рустемовна</t>
-  </si>
-  <si>
-    <t>Галиев Камиль Айратович</t>
-  </si>
-  <si>
-    <t>Шамсиев Эльдар Халилович</t>
-  </si>
-  <si>
-    <t>Гайнуллин Ильнур Ильхамович</t>
-  </si>
-  <si>
-    <t>Чукашов Вячеслав Николаевич</t>
-  </si>
-  <si>
-    <t>Махмутов Амир Фаридович</t>
-  </si>
-  <si>
-    <t>Лисицких Вероника Валериановна</t>
-  </si>
-  <si>
-    <t>Шайдуллин Никита Рустемович</t>
-  </si>
-  <si>
-    <t>Ахметзянов Ренат Ибрагимович</t>
-  </si>
-  <si>
-    <t>Соколова Юлия Алексеевна</t>
-  </si>
-  <si>
-    <t>Ларионов Алексей Андреевич</t>
-  </si>
-  <si>
-    <t>Петряев Вадим Витальевич</t>
-  </si>
-  <si>
-    <t>Пискунов Дмитрий Андреевич</t>
-  </si>
-  <si>
-    <t>Бауличева Кристина Викторовна</t>
-  </si>
-  <si>
-    <t>Хабирзянова Ралина Разиловна</t>
-  </si>
-  <si>
-    <t>Галимзянов Руслан Рефатович</t>
-  </si>
-  <si>
-    <t>Шамсутдинов Ранис Рамилевич</t>
-  </si>
-  <si>
-    <t>Ханипова Регина Рамилевна</t>
-  </si>
-  <si>
-    <t>Замалеева Гузель Ринатовна</t>
-  </si>
-  <si>
-    <t>Гайфуллин Илдус Миннахматович</t>
-  </si>
-  <si>
-    <t>Мисбахов Рустам Шаукатович</t>
-  </si>
-  <si>
-    <t>Салихов Ильнар Рамилевич</t>
-  </si>
-  <si>
-    <t>Емельянов Дмитрий Владимирович</t>
-  </si>
-  <si>
-    <t>Мокшин Владимир Васильевич</t>
-  </si>
-  <si>
-    <t>Сайфудинов Ильдар Рифатович</t>
-  </si>
-  <si>
-    <t>Сарачева Диана Азатовна</t>
-  </si>
-  <si>
-    <t>Шипилова Ольга Александровна</t>
-  </si>
-  <si>
-    <t>Хасаншина Эльвира Маратовна</t>
-  </si>
-  <si>
-    <t>Минкин Марат Риналович</t>
-  </si>
-  <si>
-    <t>Ильин Алексей Николаевич</t>
-  </si>
-  <si>
-    <t>Ахметзянов Айнур Фагилевич</t>
-  </si>
-  <si>
     <t>Астафьев Олег Валерьевич</t>
   </si>
   <si>
@@ -208,123 +208,168 @@
     <t>Юдин Павел Валентинович</t>
   </si>
   <si>
+    <t>Емельянов Денис Викторович</t>
+  </si>
+  <si>
+    <t>Ямалиева Альбина Гумаровна</t>
+  </si>
+  <si>
+    <t>Костылева Анна Николаевна</t>
+  </si>
+  <si>
+    <t>Шамсутдинов Рустам Салатович</t>
+  </si>
+  <si>
+    <t>Гаптрахимова Юлия Ринатовна</t>
+  </si>
+  <si>
+    <t>Ларионов Дмитрий Николаевич</t>
+  </si>
+  <si>
+    <t>Горшенин Ивани Викторович</t>
+  </si>
+  <si>
+    <t>Шамаев Сергей Николаевич</t>
+  </si>
+  <si>
+    <t>Мочелевская Елена Владимировна</t>
+  </si>
+  <si>
+    <t>Исаев Руслан Алиевич</t>
+  </si>
+  <si>
+    <t>Кутлакова Ильвира Наилевна</t>
+  </si>
+  <si>
+    <t>Сафаргалиев Айнур Маратович</t>
+  </si>
+  <si>
+    <t>Кузнецов Константин Валерьевич</t>
+  </si>
+  <si>
+    <t>Марухина Светлана Николаевна</t>
+  </si>
+  <si>
+    <t>Маликов Ямиль Айнуртович</t>
+  </si>
+  <si>
+    <t>Холщевникова Алсу Мокатдисовна</t>
+  </si>
+  <si>
+    <t>Казачкова Вероника Игоревна</t>
+  </si>
+  <si>
+    <t>Ибрагимов Искандер Салаватович</t>
+  </si>
+  <si>
+    <t>Набиуллин Ринат Хамитович</t>
+  </si>
+  <si>
+    <t>Гайсин Ильгам Ильдарович</t>
+  </si>
+  <si>
+    <t>Адгамов Артур Фаязович</t>
+  </si>
+  <si>
+    <t>Шарипов Рустам Айдарович</t>
+  </si>
+  <si>
+    <t>Хафизов Айзат Азатович</t>
+  </si>
+  <si>
+    <t>Васянин Даниил Олегович</t>
+  </si>
+  <si>
+    <t>Шигапов Руслан Ринатович</t>
+  </si>
+  <si>
+    <t>Газизов Камиль Азатович</t>
+  </si>
+  <si>
+    <t>Лупачев Кирилл Эдуардович</t>
+  </si>
+  <si>
+    <t>Андреева Анна Валерьевна</t>
+  </si>
+  <si>
+    <t>Галаутдинов Рифат Илдарович</t>
+  </si>
+  <si>
+    <t>Габдулфартов Артем Айратович</t>
+  </si>
+  <si>
+    <t>Гатауллин Шамиль Актасович</t>
+  </si>
+  <si>
+    <t>Халиков Рузиль Нафисович</t>
+  </si>
+  <si>
+    <t>Медведев Игорь Сергеевич</t>
+  </si>
+  <si>
+    <t>Насибуллин Марат Эдуардович</t>
+  </si>
+  <si>
+    <t>Никошина Надежда Васильевна</t>
+  </si>
+  <si>
+    <t>Матвеев Федор Юрьевич</t>
+  </si>
+  <si>
+    <t>Долгова Тамара Юрьевна</t>
+  </si>
+  <si>
+    <t>Очирова Гульнара Саидовна</t>
+  </si>
+  <si>
+    <t>Гайнуллина Эльза Ильхамовна</t>
+  </si>
+  <si>
+    <t>Халитова Ландыш Эльнуровна</t>
+  </si>
+  <si>
     <t>Никошин Герман Андреевич</t>
   </si>
   <si>
-    <t>Емельянов Денис Викторович</t>
-  </si>
-  <si>
-    <t>Ямалиева Альбина Гумаровна</t>
-  </si>
-  <si>
-    <t>Костылева Анна Николаевна</t>
-  </si>
-  <si>
-    <t>Шамсутдинов Рустам Салатович</t>
-  </si>
-  <si>
-    <t>Гаптрахимова Юлия Ринатовна</t>
-  </si>
-  <si>
-    <t>Ларионов Дмитрий Николаевич</t>
-  </si>
-  <si>
-    <t>Горшенин Ивани Викторович</t>
-  </si>
-  <si>
-    <t>Шамаев Сергей Николаевич</t>
-  </si>
-  <si>
-    <t>Мочелевская Елена Владимировна</t>
-  </si>
-  <si>
-    <t>Исаев Руслан Алиевич</t>
-  </si>
-  <si>
-    <t>Кутлакова Ильвира Наилевна</t>
-  </si>
-  <si>
-    <t>Сафаргалиев Айнур Маратович</t>
-  </si>
-  <si>
-    <t>Кузнецов Константин Валерьевич</t>
-  </si>
-  <si>
-    <t>Марухина Светлана Николаевна</t>
-  </si>
-  <si>
-    <t>Маликов Ямиль Айнуртович</t>
-  </si>
-  <si>
-    <t>Холщевникова Алсу Мокатдисовна</t>
-  </si>
-  <si>
     <t>Авзалов Булат Айратович</t>
   </si>
   <si>
-    <t>Казачкова Вероника Игоревна</t>
-  </si>
-  <si>
-    <t>Ибрагимов Искандер Салаватович</t>
-  </si>
-  <si>
-    <t>Набиуллин Ринат Хамитович</t>
-  </si>
-  <si>
-    <t>Гайсин Ильгам Ильдарович</t>
-  </si>
-  <si>
-    <t>Адгамов Артур Фаязович</t>
-  </si>
-  <si>
-    <t>Шарипов Рустам Айдарович</t>
-  </si>
-  <si>
-    <t>Хафизов Айзат Азатович</t>
-  </si>
-  <si>
-    <t>Васянин Даниил Олегович</t>
-  </si>
-  <si>
-    <t>Шигапов Руслан Ринатович</t>
+    <t>Галиев Самуил Ильнурович</t>
+  </si>
+  <si>
+    <t>Сайфутдинов Рустам Рамилевич</t>
+  </si>
+  <si>
+    <t>Гильметдинов Инсаф Нафисович</t>
+  </si>
+  <si>
+    <t>Калматова Карима Искандеровна</t>
+  </si>
+  <si>
+    <t>Герасимова Ольга Юрьевна</t>
+  </si>
+  <si>
+    <t>Хайбрахманов рамис ильгизович</t>
+  </si>
+  <si>
+    <t>Митрофанов Сергей Александрович</t>
+  </si>
+  <si>
+    <t>Валиуллин Динар Джамилович</t>
+  </si>
+  <si>
+    <t>Комиссаров Егор Сергеевич</t>
+  </si>
+  <si>
+    <t>Юнусова Алсу Ревалевна</t>
+  </si>
+  <si>
+    <t>Ахтямова Зухра Анваровна</t>
   </si>
   <si>
     <t>Мифтахов Айнур Дамирович</t>
   </si>
   <si>
-    <t>Газизов Камиль Азатович</t>
-  </si>
-  <si>
-    <t>Лупачев Кирилл Эдуардович</t>
-  </si>
-  <si>
-    <t>Андреева Анна Валерьевна</t>
-  </si>
-  <si>
-    <t>Галаутдинов Рифат Илдарович</t>
-  </si>
-  <si>
-    <t>Габдулфартов Артем Айратович</t>
-  </si>
-  <si>
-    <t>Гатауллин Шамиль Актасович</t>
-  </si>
-  <si>
-    <t>Халиков Рузиль Нафисович</t>
-  </si>
-  <si>
-    <t>Медведев Игорь Сергеевич</t>
-  </si>
-  <si>
-    <t>Насибуллин Марат Эдуардович</t>
-  </si>
-  <si>
-    <t>Никошина Надежда Васильевна</t>
-  </si>
-  <si>
-    <t>Гильметдинов Инсаф Нафисович</t>
-  </si>
-  <si>
     <t>astafev-oleg96@mail.ru</t>
   </si>
   <si>
@@ -349,87 +394,132 @@
     <t>shigapov.ruslan2011@yandex.ru</t>
   </si>
   <si>
+    <t>Kamil.g.23@yandex.ru</t>
+  </si>
+  <si>
+    <t>lupachev_2002@mail.ru</t>
+  </si>
+  <si>
+    <t>andra-85@mail.ru</t>
+  </si>
+  <si>
+    <t>it.galautdinov@gmail.com</t>
+  </si>
+  <si>
+    <t>agabdulfartov@gmail.com</t>
+  </si>
+  <si>
+    <t>nubsairacks3@mail.ru</t>
+  </si>
+  <si>
+    <t>ruzil.khalikov.020508@mail.ru</t>
+  </si>
+  <si>
+    <t>igor.medvedev2015@gmail.com</t>
+  </si>
+  <si>
+    <t>nasibullinmarat540@gmail.com</t>
+  </si>
+  <si>
+    <t>hoz-dep@alf-kai.rualf</t>
+  </si>
+  <si>
+    <t>fedmat9@gmail.com</t>
+  </si>
+  <si>
+    <t>security@alf-kai.ru</t>
+  </si>
+  <si>
+    <t>bufet@alf-kai.ru</t>
+  </si>
+  <si>
+    <t>egajnullina44@gmail.com</t>
+  </si>
+  <si>
+    <t>nandi986513@gmail.com</t>
+  </si>
+  <si>
+    <t>samuilgaliev@gmail.com</t>
+  </si>
+  <si>
+    <t>14_karrat@mail.ru</t>
+  </si>
+  <si>
+    <t>nobeliylord@gmail.com</t>
+  </si>
+  <si>
+    <t>karimakalmatova51557@gmail.com</t>
+  </si>
+  <si>
+    <t>gerola1970@mail.ru</t>
+  </si>
+  <si>
+    <t>ramis.khaybrakhmanov@mail.ru</t>
+  </si>
+  <si>
+    <t>S.mitrofanov1982@mail.ru</t>
+  </si>
+  <si>
+    <t>dinarvaliullin077@gmail.com</t>
+  </si>
+  <si>
+    <t>salafanovii.paket@mail.ru</t>
+  </si>
+  <si>
+    <t>alsuunusova7@gmail.com</t>
+  </si>
+  <si>
+    <t>zuhra_knitu@mail.ru</t>
+  </si>
+  <si>
     <t>ainur.miftahov2018@mail.ru</t>
   </si>
   <si>
-    <t>Kamil.g.23@yandex.ru</t>
-  </si>
-  <si>
-    <t>lupachev_2002@mail.ru</t>
-  </si>
-  <si>
-    <t>andra-85@mail.ru</t>
-  </si>
-  <si>
-    <t>it.galautdinov@gmail.com</t>
-  </si>
-  <si>
-    <t>agabdulfartov@gmail.com</t>
-  </si>
-  <si>
-    <t>nubsairacks3@mail.ru</t>
-  </si>
-  <si>
-    <t>ruzil.khalikov.020508@mail.ru</t>
-  </si>
-  <si>
-    <t>igor.medvedev2015@gmail.com</t>
-  </si>
-  <si>
-    <t>nasibullinmarat540@gmail.com</t>
-  </si>
-  <si>
-    <t>hoz-dep@alf-kai.rualf</t>
-  </si>
-  <si>
-    <t>nobeliylord@gmail.com</t>
-  </si>
-  <si>
     <t>22-11</t>
   </si>
   <si>
+    <t>22-81</t>
+  </si>
+  <si>
+    <t>21-02</t>
+  </si>
+  <si>
+    <t>21-05</t>
+  </si>
+  <si>
+    <t>20-07</t>
+  </si>
+  <si>
+    <t>20-00</t>
+  </si>
+  <si>
+    <t>20-02</t>
+  </si>
+  <si>
+    <t>22-05</t>
+  </si>
+  <si>
+    <t>22-03</t>
+  </si>
+  <si>
+    <t>21-85</t>
+  </si>
+  <si>
+    <t>21-00</t>
+  </si>
+  <si>
+    <t>19-07</t>
+  </si>
+  <si>
+    <t>22-76</t>
+  </si>
+  <si>
+    <t>20-05</t>
+  </si>
+  <si>
     <t>21-01</t>
   </si>
   <si>
-    <t>22-81</t>
-  </si>
-  <si>
-    <t>21-02</t>
-  </si>
-  <si>
-    <t>21-05</t>
-  </si>
-  <si>
-    <t>20-07</t>
-  </si>
-  <si>
-    <t>20-00</t>
-  </si>
-  <si>
-    <t>20-02</t>
-  </si>
-  <si>
-    <t>22-05</t>
-  </si>
-  <si>
-    <t>22-03</t>
-  </si>
-  <si>
-    <t>21-85</t>
-  </si>
-  <si>
-    <t>21-00</t>
-  </si>
-  <si>
-    <t>19-07</t>
-  </si>
-  <si>
-    <t>22-76</t>
-  </si>
-  <si>
-    <t>20-05</t>
-  </si>
-  <si>
     <t>22-00</t>
   </si>
   <si>
@@ -451,228 +541,252 @@
     <t>Сотрудник</t>
   </si>
   <si>
+    <t>Диратизация</t>
+  </si>
+  <si>
+    <t>Сотрудник(убор)</t>
+  </si>
+  <si>
+    <t>Кафедра ЕНДИТ</t>
+  </si>
+  <si>
+    <t>Представитель Газпром</t>
+  </si>
+  <si>
+    <t>Водитель</t>
+  </si>
+  <si>
+    <t>преподаватель</t>
+  </si>
+  <si>
+    <t>Рабочий</t>
+  </si>
+  <si>
+    <t>24302</t>
+  </si>
+  <si>
+    <t>24202</t>
+  </si>
+  <si>
+    <t>Уборщица</t>
+  </si>
+  <si>
+    <t>24400</t>
+  </si>
+  <si>
+    <t>24200</t>
+  </si>
+  <si>
+    <t>24111</t>
+  </si>
+  <si>
+    <t>24102</t>
+  </si>
+  <si>
+    <t>24205</t>
+  </si>
+  <si>
+    <t>24211</t>
+  </si>
+  <si>
+    <t>24405</t>
+  </si>
+  <si>
+    <t>24100</t>
+  </si>
+  <si>
+    <t>АХО</t>
+  </si>
+  <si>
+    <t>Охрана - КПП</t>
+  </si>
+  <si>
+    <t>Буфет</t>
+  </si>
+  <si>
+    <t>24105</t>
+  </si>
+  <si>
+    <t>24210</t>
+  </si>
+  <si>
     <t>ахо</t>
   </si>
   <si>
-    <t>Диратизация</t>
-  </si>
-  <si>
-    <t>Сотрудник(убор)</t>
-  </si>
-  <si>
-    <t>Кафедра ЕНДИТ</t>
-  </si>
-  <si>
-    <t>Представитель Газпром</t>
-  </si>
-  <si>
-    <t>Водитель</t>
-  </si>
-  <si>
-    <t>преподаватель</t>
-  </si>
-  <si>
-    <t>Рабочий</t>
-  </si>
-  <si>
-    <t>24302</t>
-  </si>
-  <si>
-    <t>24202</t>
-  </si>
-  <si>
-    <t>Уборщица</t>
-  </si>
-  <si>
     <t>24181</t>
   </si>
   <si>
-    <t>24400</t>
-  </si>
-  <si>
-    <t>24200</t>
-  </si>
-  <si>
-    <t>24111</t>
-  </si>
-  <si>
-    <t>24102</t>
-  </si>
-  <si>
-    <t>24205</t>
-  </si>
-  <si>
-    <t>24211</t>
-  </si>
-  <si>
-    <t>24100</t>
-  </si>
-  <si>
-    <t>24405</t>
-  </si>
-  <si>
-    <t>АХО</t>
+    <t>24381</t>
+  </si>
+  <si>
+    <t>АПК</t>
+  </si>
+  <si>
+    <t>КМТ24202</t>
+  </si>
+  <si>
+    <t>24281</t>
   </si>
   <si>
     <t>9370417998</t>
   </si>
   <si>
+    <t>90271988881</t>
+  </si>
+  <si>
+    <t>9503184734</t>
+  </si>
+  <si>
+    <t>9061203696</t>
+  </si>
+  <si>
+    <t>9172447740</t>
+  </si>
+  <si>
+    <t>9393330757</t>
+  </si>
+  <si>
+    <t>9046624590</t>
+  </si>
+  <si>
+    <t>9393935595</t>
+  </si>
+  <si>
+    <t>9046695973</t>
+  </si>
+  <si>
+    <t>9274648299</t>
+  </si>
+  <si>
+    <t>9510609003</t>
+  </si>
+  <si>
+    <t>9518965445</t>
+  </si>
+  <si>
+    <t>9867182722</t>
+  </si>
+  <si>
+    <t>9196248925</t>
+  </si>
+  <si>
+    <t>9196374658</t>
+  </si>
+  <si>
+    <t>9172617001</t>
+  </si>
+  <si>
+    <t>9393143898</t>
+  </si>
+  <si>
+    <t>9178760484</t>
+  </si>
+  <si>
+    <t>9179259416</t>
+  </si>
+  <si>
+    <t>9534935723</t>
+  </si>
+  <si>
+    <t>9505261873</t>
+  </si>
+  <si>
+    <t>9674671710</t>
+  </si>
+  <si>
+    <t>9083384423</t>
+  </si>
+  <si>
+    <t>9172466483</t>
+  </si>
+  <si>
+    <t>9518967075</t>
+  </si>
+  <si>
+    <t>9179098585</t>
+  </si>
+  <si>
+    <t>9172552892</t>
+  </si>
+  <si>
+    <t>9179091544</t>
+  </si>
+  <si>
+    <t>9991698837</t>
+  </si>
+  <si>
+    <t>9375977380</t>
+  </si>
+  <si>
+    <t>9172960496</t>
+  </si>
+  <si>
+    <t>9274329662</t>
+  </si>
+  <si>
+    <t>9003201506</t>
+  </si>
+  <si>
+    <t>9196498411</t>
+  </si>
+  <si>
+    <t>9534935738</t>
+  </si>
+  <si>
+    <t>9518908177</t>
+  </si>
+  <si>
+    <t>9631574322</t>
+  </si>
+  <si>
+    <t>9047136971</t>
+  </si>
+  <si>
+    <t>9196962394</t>
+  </si>
+  <si>
+    <t>9179080169</t>
+  </si>
+  <si>
+    <t>9172222346</t>
+  </si>
+  <si>
+    <t>9872956973</t>
+  </si>
+  <si>
+    <t>9518965371</t>
+  </si>
+  <si>
+    <t>9600847030</t>
+  </si>
+  <si>
+    <t>9270322877</t>
+  </si>
+  <si>
+    <t>9179200106</t>
+  </si>
+  <si>
+    <t>9179223372</t>
+  </si>
+  <si>
+    <t>9173949153</t>
+  </si>
+  <si>
+    <t>9178980356</t>
+  </si>
+  <si>
+    <t>9600815730</t>
+  </si>
+  <si>
+    <t>9179025062</t>
+  </si>
+  <si>
+    <t>9872767372</t>
+  </si>
+  <si>
     <t>917259387</t>
   </si>
   <si>
-    <t>90271988881</t>
-  </si>
-  <si>
-    <t>9503184734</t>
-  </si>
-  <si>
-    <t>9061203696</t>
-  </si>
-  <si>
-    <t>9172447740</t>
-  </si>
-  <si>
-    <t>9393330757</t>
-  </si>
-  <si>
-    <t>9046624590</t>
-  </si>
-  <si>
-    <t>9393935595</t>
-  </si>
-  <si>
-    <t>9046695973</t>
-  </si>
-  <si>
-    <t>9274648299</t>
-  </si>
-  <si>
-    <t>9510609003</t>
-  </si>
-  <si>
-    <t>9518965445</t>
-  </si>
-  <si>
-    <t>9867182722</t>
-  </si>
-  <si>
-    <t>9196248925</t>
-  </si>
-  <si>
-    <t>9196374658</t>
-  </si>
-  <si>
-    <t>9172617001</t>
-  </si>
-  <si>
-    <t>9393143898</t>
-  </si>
-  <si>
-    <t>9178760484</t>
-  </si>
-  <si>
-    <t>9179259416</t>
-  </si>
-  <si>
-    <t>9534935723</t>
-  </si>
-  <si>
-    <t>9505261873</t>
-  </si>
-  <si>
-    <t>9674671710</t>
-  </si>
-  <si>
-    <t>9083384423</t>
-  </si>
-  <si>
-    <t>9172466483</t>
-  </si>
-  <si>
-    <t>9518967075</t>
-  </si>
-  <si>
-    <t>9179098585</t>
-  </si>
-  <si>
-    <t>9172552892</t>
-  </si>
-  <si>
-    <t>9179091544</t>
-  </si>
-  <si>
-    <t>9991698837</t>
-  </si>
-  <si>
-    <t>9375977380</t>
-  </si>
-  <si>
-    <t>9172960496</t>
-  </si>
-  <si>
-    <t>9274329662</t>
-  </si>
-  <si>
-    <t>9003201506</t>
-  </si>
-  <si>
-    <t>9196498411</t>
-  </si>
-  <si>
-    <t>9534935738</t>
-  </si>
-  <si>
-    <t>9518908177</t>
-  </si>
-  <si>
-    <t>9631574322</t>
-  </si>
-  <si>
-    <t>9047136971</t>
-  </si>
-  <si>
-    <t>9196962394</t>
-  </si>
-  <si>
-    <t>9179080169</t>
-  </si>
-  <si>
-    <t>9172222346</t>
-  </si>
-  <si>
-    <t>9872956973</t>
-  </si>
-  <si>
-    <t>9518965371</t>
-  </si>
-  <si>
-    <t>9600847030</t>
-  </si>
-  <si>
-    <t>9270322877</t>
-  </si>
-  <si>
-    <t>9179200106</t>
-  </si>
-  <si>
-    <t>9179223372</t>
-  </si>
-  <si>
-    <t>9173949153</t>
-  </si>
-  <si>
-    <t>9178980356</t>
-  </si>
-  <si>
-    <t>9600815730</t>
-  </si>
-  <si>
-    <t>9179025062</t>
-  </si>
-  <si>
-    <t>9872767372</t>
-  </si>
-  <si>
     <t>+79172993502</t>
   </si>
   <si>
@@ -685,129 +799,171 @@
     <t>9876543210</t>
   </si>
   <si>
+    <t>9534870186</t>
+  </si>
+  <si>
+    <t>79872314841</t>
+  </si>
+  <si>
+    <t>9196372101</t>
+  </si>
+  <si>
+    <t>79872984639</t>
+  </si>
+  <si>
+    <t>9870696164</t>
+  </si>
+  <si>
+    <t>9173931716</t>
+  </si>
+  <si>
+    <t>9172715715</t>
+  </si>
+  <si>
+    <t>9172627869</t>
+  </si>
+  <si>
+    <t>9172681515</t>
+  </si>
+  <si>
+    <t>79172549239</t>
+  </si>
+  <si>
+    <t>9520371508</t>
+  </si>
+  <si>
+    <t>79991558379</t>
+  </si>
+  <si>
+    <t>9393193082</t>
+  </si>
+  <si>
+    <t>9173959232</t>
+  </si>
+  <si>
+    <t>79996230432</t>
+  </si>
+  <si>
+    <t>9172381431</t>
+  </si>
+  <si>
+    <t>89009009009</t>
+  </si>
+  <si>
+    <t>89874885509</t>
+  </si>
+  <si>
+    <t>89172898544</t>
+  </si>
+  <si>
+    <t>89872231796</t>
+  </si>
+  <si>
+    <t>89872216876</t>
+  </si>
+  <si>
+    <t>89083432610</t>
+  </si>
+  <si>
+    <t>89393840560</t>
+  </si>
+  <si>
+    <t>89872378095</t>
+  </si>
+  <si>
+    <t>89172617052</t>
+  </si>
+  <si>
+    <t>89503200575</t>
+  </si>
+  <si>
+    <t>89872948316</t>
+  </si>
+  <si>
+    <t>89179229808</t>
+  </si>
+  <si>
+    <t>89393475969</t>
+  </si>
+  <si>
+    <t>89869187404</t>
+  </si>
+  <si>
+    <t>89872368424</t>
+  </si>
+  <si>
+    <t>89178581590</t>
+  </si>
+  <si>
+    <t>89872656316</t>
+  </si>
+  <si>
+    <t>89083343376</t>
+  </si>
+  <si>
+    <t>89179345683</t>
+  </si>
+  <si>
+    <t>89872110050</t>
+  </si>
+  <si>
+    <t>89600768750</t>
+  </si>
+  <si>
+    <t>89178872062</t>
+  </si>
+  <si>
+    <t>89600805284</t>
+  </si>
+  <si>
+    <t>79393664986</t>
+  </si>
+  <si>
     <t>9991626022</t>
   </si>
   <si>
-    <t>9534870186</t>
-  </si>
-  <si>
-    <t>79872314841</t>
-  </si>
-  <si>
-    <t>9196372101</t>
-  </si>
-  <si>
-    <t>79872984639</t>
-  </si>
-  <si>
-    <t>9870696164</t>
-  </si>
-  <si>
-    <t>9173931716</t>
-  </si>
-  <si>
-    <t>9172715715</t>
-  </si>
-  <si>
-    <t>9172627869</t>
-  </si>
-  <si>
-    <t>9172681515</t>
-  </si>
-  <si>
-    <t>79172549239</t>
-  </si>
-  <si>
-    <t>9520371508</t>
-  </si>
-  <si>
-    <t>79991558379</t>
-  </si>
-  <si>
-    <t>9393193082</t>
-  </si>
-  <si>
-    <t>9173959232</t>
-  </si>
-  <si>
-    <t>79996230432</t>
-  </si>
-  <si>
-    <t>9172381431</t>
-  </si>
-  <si>
     <t>89870610226</t>
   </si>
   <si>
-    <t>89009009009</t>
-  </si>
-  <si>
-    <t>89874885509</t>
-  </si>
-  <si>
-    <t>89172898544</t>
-  </si>
-  <si>
-    <t>89872231796</t>
-  </si>
-  <si>
-    <t>89872216876</t>
-  </si>
-  <si>
-    <t>89083432610</t>
-  </si>
-  <si>
-    <t>89393840560</t>
-  </si>
-  <si>
-    <t>89872378095</t>
-  </si>
-  <si>
-    <t>89172617052</t>
+    <t>89196957484</t>
+  </si>
+  <si>
+    <t>89179125390</t>
+  </si>
+  <si>
+    <t>+79083385215</t>
+  </si>
+  <si>
+    <t>89631222952</t>
+  </si>
+  <si>
+    <t>89600886140</t>
+  </si>
+  <si>
+    <t>79961214758</t>
+  </si>
+  <si>
+    <t>89063301362</t>
+  </si>
+  <si>
+    <t>89178893917</t>
+  </si>
+  <si>
+    <t>89172820248</t>
+  </si>
+  <si>
+    <t>89083369215</t>
+  </si>
+  <si>
+    <t>89872798161</t>
   </si>
   <si>
     <t>89372968592</t>
   </si>
   <si>
-    <t>89503200575</t>
-  </si>
-  <si>
-    <t>89872948316</t>
-  </si>
-  <si>
-    <t>89179229808</t>
-  </si>
-  <si>
-    <t>89393475969</t>
-  </si>
-  <si>
-    <t>89869187404</t>
-  </si>
-  <si>
-    <t>89872368424</t>
-  </si>
-  <si>
-    <t>89178581590</t>
-  </si>
-  <si>
-    <t>89872656316</t>
-  </si>
-  <si>
-    <t>89083343376</t>
-  </si>
-  <si>
-    <t>89179345683</t>
-  </si>
-  <si>
-    <t>+79083385215</t>
-  </si>
-  <si>
     <t>Е726ОМ/716</t>
   </si>
   <si>
-    <t>Н717ХТ|116</t>
-  </si>
-  <si>
     <t>К758АУ|716</t>
   </si>
   <si>
@@ -961,6 +1117,9 @@
     <t>О587МХ|716</t>
   </si>
   <si>
+    <t>Н503ТР|116</t>
+  </si>
+  <si>
     <t>Н632РК|716</t>
   </si>
   <si>
@@ -973,9 +1132,6 @@
     <t>Е835УО|116</t>
   </si>
   <si>
-    <t>В211НН|716</t>
-  </si>
-  <si>
     <t>К938ОХ|116</t>
   </si>
   <si>
@@ -1024,67 +1180,112 @@
     <t>К211ОС|716</t>
   </si>
   <si>
+    <t>М174СЕ|702</t>
+  </si>
+  <si>
+    <t>С812МУ|116</t>
+  </si>
+  <si>
+    <t>К205РТ|716</t>
+  </si>
+  <si>
+    <t>Е766ТР|716</t>
+  </si>
+  <si>
+    <t>Р295КТ|116</t>
+  </si>
+  <si>
+    <t>О288МО|716</t>
+  </si>
+  <si>
+    <t>Х049ВУ|116</t>
+  </si>
+  <si>
+    <t>В847КР|716</t>
+  </si>
+  <si>
+    <t>О361ТР|716</t>
+  </si>
+  <si>
+    <t>Е006СУ|116</t>
+  </si>
+  <si>
+    <t>С043ЕМ|716</t>
+  </si>
+  <si>
+    <t>А882ХХ|716</t>
+  </si>
+  <si>
+    <t>К364ТТ|716</t>
+  </si>
+  <si>
+    <t>А023УМ|116</t>
+  </si>
+  <si>
+    <t>О775ТН|716</t>
+  </si>
+  <si>
+    <t>Е651РМ|716</t>
+  </si>
+  <si>
+    <t>Т791СВ|16</t>
+  </si>
+  <si>
+    <t>Е532МО|116</t>
+  </si>
+  <si>
+    <t>Х323УА|116</t>
+  </si>
+  <si>
+    <t>A000AA|16</t>
+  </si>
+  <si>
+    <t>К906СУ|116</t>
+  </si>
+  <si>
+    <t>Р803ЕВ|116</t>
+  </si>
+  <si>
+    <t>М151НА|716</t>
+  </si>
+  <si>
     <t>У847АО|116</t>
   </si>
   <si>
-    <t>М174СЕ|702</t>
-  </si>
-  <si>
-    <t>С812МУ|116</t>
-  </si>
-  <si>
-    <t>К205РТ|716</t>
-  </si>
-  <si>
-    <t>Е766ТР|716</t>
-  </si>
-  <si>
-    <t>Р295КТ|116</t>
-  </si>
-  <si>
-    <t>О288МО|716</t>
-  </si>
-  <si>
-    <t>Х049ВУ|116</t>
-  </si>
-  <si>
-    <t>В847КР|716</t>
+    <t>М951УТ|716</t>
+  </si>
+  <si>
+    <t>О309ОР|716</t>
+  </si>
+  <si>
+    <t>A363МА|116</t>
+  </si>
+  <si>
+    <t>О546УА|716</t>
+  </si>
+  <si>
+    <t>Р503УУ|16</t>
+  </si>
+  <si>
+    <t>К809АУ|716</t>
+  </si>
+  <si>
+    <t>А397ЕО|716</t>
+  </si>
+  <si>
+    <t>М316ВХ|16</t>
+  </si>
+  <si>
+    <t>О175СМ|716</t>
+  </si>
+  <si>
+    <t>С254НВ|716</t>
+  </si>
+  <si>
+    <t>Т818ЕР|116</t>
   </si>
   <si>
     <t>А154СС|716</t>
-  </si>
-  <si>
-    <t>О361ТР|716</t>
-  </si>
-  <si>
-    <t>Е006СУ|116</t>
-  </si>
-  <si>
-    <t>С043ЕМ|716</t>
-  </si>
-  <si>
-    <t>А882ХХ|716</t>
-  </si>
-  <si>
-    <t>К364ТТ|716</t>
-  </si>
-  <si>
-    <t>А023УМ|116</t>
-  </si>
-  <si>
-    <t>О775ТН|716</t>
-  </si>
-  <si>
-    <t>Е651РМ|716</t>
-  </si>
-  <si>
-    <t>Т791СВ|16</t>
-  </si>
-  <si>
-    <t>Е532МО|116</t>
-  </si>
-  <si>
-    <t>A363МА|116</t>
   </si>
   <si>
     <t>Студент</t>
@@ -1448,7 +1649,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1485,1056 +1686,1056 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="F2" t="s">
-        <v>262</v>
+        <v>315</v>
       </c>
       <c r="G2" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>408524889</v>
+        <v>415242194</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="F3" t="s">
-        <v>263</v>
+        <v>316</v>
       </c>
       <c r="G3" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>415242194</v>
+        <v>427699001</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="F4" t="s">
-        <v>264</v>
+        <v>317</v>
       </c>
       <c r="G4" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>427699001</v>
+        <v>469895799</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
-        <v>169</v>
+        <v>207</v>
       </c>
       <c r="F5" t="s">
-        <v>265</v>
+        <v>318</v>
       </c>
       <c r="G5" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>469895799</v>
+        <v>476571353</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="E6" t="s">
-        <v>170</v>
+        <v>208</v>
       </c>
       <c r="F6" t="s">
-        <v>266</v>
+        <v>319</v>
       </c>
       <c r="G6" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>476571353</v>
+        <v>479036037</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="E7" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
       <c r="F7" t="s">
-        <v>267</v>
+        <v>320</v>
       </c>
       <c r="G7" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>479036037</v>
+        <v>490204203</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="F8" t="s">
-        <v>268</v>
+        <v>321</v>
       </c>
       <c r="G8" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>490204203</v>
+        <v>517154599</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="E9" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="F9" t="s">
-        <v>269</v>
+        <v>322</v>
       </c>
       <c r="G9" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>517154599</v>
+        <v>603136495</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="E10" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="F10" t="s">
-        <v>270</v>
+        <v>323</v>
       </c>
       <c r="G10" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>603136495</v>
+        <v>718944986</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="E11" t="s">
-        <v>175</v>
+        <v>213</v>
       </c>
       <c r="F11" t="s">
-        <v>271</v>
+        <v>324</v>
       </c>
       <c r="G11" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>718944986</v>
+        <v>720436821</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="E12" t="s">
-        <v>176</v>
+        <v>214</v>
       </c>
       <c r="F12" t="s">
-        <v>272</v>
+        <v>325</v>
       </c>
       <c r="G12" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
-        <v>720436821</v>
+        <v>740142002</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F13" t="s">
-        <v>273</v>
+        <v>326</v>
       </c>
       <c r="G13" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>740142002</v>
+        <v>746664360</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="E14" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="F14" t="s">
-        <v>274</v>
+        <v>327</v>
       </c>
       <c r="G14" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>746664360</v>
+        <v>761493593</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="E15" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="F15" t="s">
-        <v>275</v>
+        <v>328</v>
       </c>
       <c r="G15" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>761493593</v>
+        <v>774097707</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="E16" t="s">
-        <v>180</v>
+        <v>218</v>
       </c>
       <c r="F16" t="s">
-        <v>276</v>
+        <v>329</v>
       </c>
       <c r="G16" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>774097707</v>
+        <v>785422208</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="E17" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
       <c r="F17" t="s">
-        <v>277</v>
+        <v>330</v>
       </c>
       <c r="G17" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
-        <v>785422208</v>
+        <v>840380591</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="F18" t="s">
-        <v>278</v>
+        <v>331</v>
       </c>
       <c r="G18" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
-        <v>840380591</v>
+        <v>862027267</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="E19" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="F19" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
       <c r="G19" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20">
-        <v>862027267</v>
+        <v>874085109</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="E20" t="s">
-        <v>184</v>
+        <v>222</v>
       </c>
       <c r="F20" t="s">
-        <v>280</v>
+        <v>333</v>
       </c>
       <c r="G20" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21">
-        <v>874085109</v>
+        <v>915217913</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="E21" t="s">
-        <v>185</v>
+        <v>223</v>
       </c>
       <c r="F21" t="s">
-        <v>281</v>
+        <v>334</v>
       </c>
       <c r="G21" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22">
-        <v>915217913</v>
+        <v>942266011</v>
       </c>
       <c r="B22" t="s">
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="E22" t="s">
-        <v>186</v>
+        <v>224</v>
       </c>
       <c r="F22" t="s">
-        <v>282</v>
+        <v>335</v>
       </c>
       <c r="G22" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23">
-        <v>942266011</v>
+        <v>953371377</v>
       </c>
       <c r="B23" t="s">
         <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="E23" t="s">
-        <v>187</v>
+        <v>225</v>
       </c>
       <c r="F23" t="s">
-        <v>283</v>
+        <v>336</v>
       </c>
       <c r="G23" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
-        <v>953371377</v>
+        <v>1019737485</v>
       </c>
       <c r="B24" t="s">
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="E24" t="s">
-        <v>188</v>
+        <v>226</v>
       </c>
       <c r="F24" t="s">
-        <v>284</v>
+        <v>337</v>
       </c>
       <c r="G24" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
-        <v>1019737485</v>
+        <v>1110388277</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="E25" t="s">
-        <v>189</v>
+        <v>227</v>
       </c>
       <c r="F25" t="s">
-        <v>285</v>
+        <v>338</v>
       </c>
       <c r="G25" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
-        <v>1110388277</v>
+        <v>1112760211</v>
       </c>
       <c r="B26" t="s">
         <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="E26" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="F26" t="s">
-        <v>286</v>
+        <v>339</v>
       </c>
       <c r="G26" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
-        <v>1112760211</v>
+        <v>1126502310</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="E27" t="s">
-        <v>191</v>
+        <v>229</v>
       </c>
       <c r="F27" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="G27" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>1126502310</v>
+        <v>1147999326</v>
       </c>
       <c r="B28" t="s">
         <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="E28" t="s">
-        <v>192</v>
+        <v>230</v>
       </c>
       <c r="F28" t="s">
-        <v>288</v>
+        <v>341</v>
       </c>
       <c r="G28" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
-        <v>1147999326</v>
+        <v>1225305929</v>
       </c>
       <c r="B29" t="s">
         <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="E29" t="s">
-        <v>193</v>
+        <v>231</v>
       </c>
       <c r="F29" t="s">
-        <v>289</v>
+        <v>342</v>
       </c>
       <c r="G29" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
-        <v>1225305929</v>
+        <v>1387773671</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="E30" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="F30" t="s">
-        <v>290</v>
+        <v>343</v>
       </c>
       <c r="G30" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
-        <v>1387773671</v>
+        <v>1427045808</v>
       </c>
       <c r="B31" t="s">
         <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="E31" t="s">
-        <v>195</v>
+        <v>233</v>
       </c>
       <c r="F31" t="s">
-        <v>291</v>
+        <v>344</v>
       </c>
       <c r="G31" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32">
-        <v>1427045808</v>
+        <v>1637708423</v>
       </c>
       <c r="B32" t="s">
         <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="E32" t="s">
-        <v>196</v>
+        <v>234</v>
       </c>
       <c r="F32" t="s">
-        <v>292</v>
+        <v>345</v>
       </c>
       <c r="G32" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33">
-        <v>1637708423</v>
+        <v>1703776173</v>
       </c>
       <c r="B33" t="s">
         <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
+        <v>168</v>
       </c>
       <c r="E33" t="s">
-        <v>197</v>
+        <v>235</v>
       </c>
       <c r="F33" t="s">
-        <v>293</v>
+        <v>346</v>
       </c>
       <c r="G33" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
-        <v>1703776173</v>
+        <v>2029961346</v>
       </c>
       <c r="B34" t="s">
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="E34" t="s">
-        <v>198</v>
+        <v>236</v>
       </c>
       <c r="F34" t="s">
-        <v>294</v>
+        <v>347</v>
       </c>
       <c r="G34" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
-        <v>2029961346</v>
+        <v>2074708631</v>
       </c>
       <c r="B35" t="s">
         <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="E35" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="F35" t="s">
-        <v>295</v>
+        <v>348</v>
       </c>
       <c r="G35" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
-        <v>2074708631</v>
+        <v>5095591691</v>
       </c>
       <c r="B36" t="s">
         <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="E36" t="s">
-        <v>200</v>
+        <v>238</v>
       </c>
       <c r="F36" t="s">
-        <v>296</v>
+        <v>349</v>
       </c>
       <c r="G36" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37">
-        <v>5095591691</v>
+        <v>5101088417</v>
       </c>
       <c r="B37" t="s">
         <v>42</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="E37" t="s">
-        <v>201</v>
+        <v>239</v>
       </c>
       <c r="F37" t="s">
-        <v>297</v>
+        <v>350</v>
       </c>
       <c r="G37" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38">
-        <v>5101088417</v>
+        <v>5162707237</v>
       </c>
       <c r="B38" t="s">
         <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="E38" t="s">
-        <v>202</v>
+        <v>240</v>
       </c>
       <c r="F38" t="s">
-        <v>298</v>
+        <v>351</v>
       </c>
       <c r="G38" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39">
-        <v>5162707237</v>
+        <v>5238994183</v>
       </c>
       <c r="B39" t="s">
         <v>44</v>
       </c>
       <c r="D39" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="E39" t="s">
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="F39" t="s">
-        <v>299</v>
+        <v>352</v>
       </c>
       <c r="G39" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40">
-        <v>5238994183</v>
+        <v>5377231472</v>
       </c>
       <c r="B40" t="s">
         <v>45</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="E40" t="s">
-        <v>204</v>
+        <v>242</v>
       </c>
       <c r="F40" t="s">
-        <v>300</v>
+        <v>353</v>
       </c>
       <c r="G40" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41">
-        <v>5377231472</v>
+        <v>5416782436</v>
       </c>
       <c r="B41" t="s">
         <v>46</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="E41" t="s">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="F41" t="s">
-        <v>301</v>
+        <v>354</v>
       </c>
       <c r="G41" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42">
-        <v>5416782436</v>
+        <v>245961900</v>
       </c>
       <c r="B42" t="s">
         <v>47</v>
       </c>
       <c r="D42" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="E42" t="s">
-        <v>206</v>
+        <v>244</v>
       </c>
       <c r="F42" t="s">
-        <v>302</v>
+        <v>355</v>
       </c>
       <c r="G42" t="s">
-        <v>357</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43">
-        <v>245961900</v>
+        <v>331732440</v>
       </c>
       <c r="B43" t="s">
         <v>48</v>
       </c>
       <c r="D43" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E43" t="s">
-        <v>207</v>
+        <v>245</v>
       </c>
       <c r="F43" t="s">
-        <v>303</v>
+        <v>356</v>
       </c>
       <c r="G43" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44">
-        <v>331732440</v>
+        <v>768759916</v>
       </c>
       <c r="B44" t="s">
         <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E44" t="s">
-        <v>208</v>
+        <v>246</v>
       </c>
       <c r="F44" t="s">
-        <v>304</v>
+        <v>357</v>
       </c>
       <c r="G44" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45">
-        <v>768759916</v>
+        <v>809691999</v>
       </c>
       <c r="B45" t="s">
         <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E45" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="F45" t="s">
-        <v>305</v>
+        <v>358</v>
       </c>
       <c r="G45" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46">
-        <v>809691999</v>
+        <v>931611739</v>
       </c>
       <c r="B46" t="s">
         <v>51</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E46" t="s">
-        <v>210</v>
+        <v>248</v>
       </c>
       <c r="F46" t="s">
-        <v>306</v>
+        <v>359</v>
       </c>
       <c r="G46" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47">
-        <v>931611739</v>
+        <v>1130245307</v>
       </c>
       <c r="B47" t="s">
         <v>52</v>
       </c>
       <c r="D47" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E47" t="s">
-        <v>211</v>
+        <v>249</v>
       </c>
       <c r="F47" t="s">
-        <v>307</v>
+        <v>360</v>
       </c>
       <c r="G47" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48">
-        <v>1130245307</v>
+        <v>1458989435</v>
       </c>
       <c r="B48" t="s">
         <v>53</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E48" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="F48" t="s">
-        <v>308</v>
+        <v>361</v>
       </c>
       <c r="G48" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49">
-        <v>1458989435</v>
+        <v>1535853897</v>
       </c>
       <c r="B49" t="s">
         <v>54</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E49" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F49" t="s">
-        <v>309</v>
+        <v>362</v>
       </c>
       <c r="G49" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50">
-        <v>1535853897</v>
+        <v>1619306377</v>
       </c>
       <c r="B50" t="s">
         <v>55</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E50" t="s">
-        <v>214</v>
+        <v>252</v>
       </c>
       <c r="F50" t="s">
-        <v>310</v>
+        <v>363</v>
       </c>
       <c r="G50" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51">
-        <v>1619306377</v>
+        <v>5124347679</v>
       </c>
       <c r="B51" t="s">
         <v>56</v>
       </c>
       <c r="D51" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E51" t="s">
-        <v>215</v>
+        <v>253</v>
       </c>
       <c r="F51" t="s">
-        <v>311</v>
+        <v>364</v>
       </c>
       <c r="G51" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52">
-        <v>5124347679</v>
+        <v>5195433855</v>
       </c>
       <c r="B52" t="s">
         <v>57</v>
       </c>
       <c r="D52" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E52" t="s">
-        <v>216</v>
+        <v>254</v>
       </c>
       <c r="F52" t="s">
-        <v>312</v>
+        <v>365</v>
       </c>
       <c r="G52" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53">
-        <v>5195433855</v>
+        <v>753366106</v>
       </c>
       <c r="B53" t="s">
         <v>58</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="E53" t="s">
-        <v>217</v>
+        <v>255</v>
       </c>
       <c r="F53" t="s">
-        <v>313</v>
+        <v>366</v>
       </c>
       <c r="G53" t="s">
-        <v>141</v>
+        <v>424</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54">
-        <v>753366106</v>
+        <v>408524889</v>
       </c>
       <c r="B54" t="s">
         <v>59</v>
       </c>
       <c r="D54" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="E54" t="s">
-        <v>218</v>
+        <v>256</v>
       </c>
       <c r="F54" t="s">
-        <v>314</v>
+        <v>367</v>
       </c>
       <c r="G54" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2545,19 +2746,19 @@
         <v>60</v>
       </c>
       <c r="C55" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="E55" t="s">
-        <v>219</v>
+        <v>257</v>
       </c>
       <c r="F55" t="s">
-        <v>315</v>
+        <v>368</v>
       </c>
       <c r="G55" t="s">
-        <v>358</v>
+        <v>425</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2568,16 +2769,16 @@
         <v>61</v>
       </c>
       <c r="D56" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E56" t="s">
-        <v>220</v>
+        <v>258</v>
       </c>
       <c r="F56" t="s">
-        <v>316</v>
+        <v>369</v>
       </c>
       <c r="G56" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2588,16 +2789,16 @@
         <v>62</v>
       </c>
       <c r="D57" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="E57" t="s">
-        <v>221</v>
+        <v>259</v>
       </c>
       <c r="F57" t="s">
-        <v>317</v>
+        <v>370</v>
       </c>
       <c r="G57" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2608,853 +2809,1198 @@
         <v>63</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="E58" t="s">
-        <v>222</v>
+        <v>260</v>
       </c>
       <c r="F58" t="s">
-        <v>318</v>
+        <v>371</v>
       </c>
       <c r="G58" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59">
-        <v>791160917</v>
+        <v>902612902</v>
       </c>
       <c r="B59" t="s">
         <v>64</v>
       </c>
       <c r="D59" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="E59" t="s">
-        <v>223</v>
+        <v>261</v>
       </c>
       <c r="F59" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="G59" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60">
-        <v>902612902</v>
+        <v>1291942039</v>
       </c>
       <c r="B60" t="s">
         <v>65</v>
       </c>
       <c r="D60" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="E60" t="s">
-        <v>224</v>
+        <v>262</v>
       </c>
       <c r="F60" t="s">
-        <v>320</v>
+        <v>373</v>
       </c>
       <c r="G60" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61">
-        <v>1291942039</v>
+        <v>1416399275</v>
       </c>
       <c r="B61" t="s">
         <v>66</v>
       </c>
       <c r="D61" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="E61" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
       <c r="F61" t="s">
-        <v>321</v>
+        <v>374</v>
       </c>
       <c r="G61" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62">
-        <v>1416399275</v>
+        <v>1688833286</v>
       </c>
       <c r="B62" t="s">
         <v>67</v>
       </c>
       <c r="D62" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="E62" t="s">
-        <v>226</v>
+        <v>264</v>
       </c>
       <c r="F62" t="s">
-        <v>322</v>
+        <v>375</v>
       </c>
       <c r="G62" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63">
-        <v>1688833286</v>
+        <v>1749600719</v>
       </c>
       <c r="B63" t="s">
         <v>68</v>
       </c>
       <c r="D63" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="E63" t="s">
-        <v>227</v>
+        <v>265</v>
       </c>
       <c r="F63" t="s">
-        <v>323</v>
+        <v>376</v>
       </c>
       <c r="G63" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64">
-        <v>1749600719</v>
+        <v>1760377606</v>
       </c>
       <c r="B64" t="s">
         <v>69</v>
       </c>
       <c r="D64" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="E64" t="s">
-        <v>228</v>
+        <v>266</v>
       </c>
       <c r="F64" t="s">
-        <v>324</v>
+        <v>377</v>
       </c>
       <c r="G64" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65">
-        <v>1760377606</v>
+        <v>5147498731</v>
       </c>
       <c r="B65" t="s">
         <v>70</v>
       </c>
       <c r="D65" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
       <c r="E65" t="s">
-        <v>229</v>
+        <v>267</v>
       </c>
       <c r="F65" t="s">
-        <v>325</v>
+        <v>378</v>
       </c>
       <c r="G65" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66">
-        <v>5147498731</v>
+        <v>5151839157</v>
       </c>
       <c r="B66" t="s">
         <v>71</v>
       </c>
       <c r="D66" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="E66" t="s">
-        <v>230</v>
+        <v>268</v>
       </c>
       <c r="F66" t="s">
-        <v>326</v>
+        <v>379</v>
       </c>
       <c r="G66" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67">
-        <v>5151839157</v>
+        <v>5266182167</v>
       </c>
       <c r="B67" t="s">
         <v>72</v>
       </c>
       <c r="D67" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="E67" t="s">
-        <v>231</v>
+        <v>269</v>
       </c>
       <c r="F67" t="s">
-        <v>327</v>
+        <v>380</v>
       </c>
       <c r="G67" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68">
-        <v>5266182167</v>
+        <v>5273682340</v>
       </c>
       <c r="B68" t="s">
         <v>73</v>
       </c>
       <c r="D68" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="E68" t="s">
-        <v>232</v>
+        <v>270</v>
       </c>
       <c r="F68" t="s">
-        <v>328</v>
+        <v>381</v>
       </c>
       <c r="G68" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69">
-        <v>5273682340</v>
+        <v>5288673453</v>
       </c>
       <c r="B69" t="s">
         <v>74</v>
       </c>
       <c r="D69" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="E69" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="F69" t="s">
-        <v>329</v>
+        <v>382</v>
       </c>
       <c r="G69" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70">
-        <v>5288673453</v>
+        <v>5296944422</v>
       </c>
       <c r="B70" t="s">
         <v>75</v>
       </c>
       <c r="D70" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="E70" t="s">
-        <v>234</v>
+        <v>272</v>
       </c>
       <c r="F70" t="s">
-        <v>330</v>
+        <v>383</v>
       </c>
       <c r="G70" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71">
-        <v>5296944422</v>
+        <v>5489771264</v>
       </c>
       <c r="B71" t="s">
         <v>76</v>
       </c>
       <c r="D71" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="E71" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F71" t="s">
-        <v>331</v>
+        <v>384</v>
       </c>
       <c r="G71" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72">
-        <v>5489771264</v>
+        <v>5536434183</v>
       </c>
       <c r="B72" t="s">
         <v>77</v>
       </c>
       <c r="D72" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="E72" t="s">
-        <v>236</v>
+        <v>274</v>
       </c>
       <c r="F72" t="s">
-        <v>332</v>
+        <v>385</v>
       </c>
       <c r="G72" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73">
-        <v>5536434183</v>
+        <v>5577684669</v>
       </c>
       <c r="B73" t="s">
         <v>78</v>
       </c>
       <c r="D73" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="E73" t="s">
-        <v>237</v>
+        <v>275</v>
       </c>
       <c r="F73" t="s">
-        <v>333</v>
+        <v>386</v>
       </c>
       <c r="G73" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74">
-        <v>5577684669</v>
+        <v>5799598774</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
       </c>
       <c r="D74" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="E74" t="s">
-        <v>238</v>
+        <v>276</v>
       </c>
       <c r="F74" t="s">
-        <v>334</v>
+        <v>387</v>
       </c>
       <c r="G74" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75">
-        <v>5799598774</v>
+        <v>1078837711</v>
       </c>
       <c r="B75" t="s">
         <v>80</v>
       </c>
       <c r="D75" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="E75" t="s">
-        <v>239</v>
+        <v>277</v>
       </c>
       <c r="F75" t="s">
-        <v>335</v>
+        <v>368</v>
       </c>
       <c r="G75" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76">
-        <v>1499636883</v>
+        <v>855809616</v>
       </c>
       <c r="B76" t="s">
         <v>81</v>
       </c>
       <c r="D76" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="E76" t="s">
-        <v>240</v>
+        <v>278</v>
       </c>
       <c r="F76" t="s">
-        <v>336</v>
+        <v>388</v>
       </c>
       <c r="G76" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77">
-        <v>1078837711</v>
+        <v>1299680937</v>
       </c>
       <c r="B77" t="s">
         <v>82</v>
       </c>
+      <c r="C77" t="s">
+        <v>119</v>
+      </c>
       <c r="D77" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="E77" t="s">
-        <v>241</v>
+        <v>279</v>
       </c>
       <c r="F77" t="s">
-        <v>315</v>
+        <v>389</v>
       </c>
       <c r="G77" t="s">
-        <v>144</v>
+        <v>424</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78">
-        <v>855809616</v>
+        <v>779497488</v>
       </c>
       <c r="B78" t="s">
         <v>83</v>
       </c>
+      <c r="C78" t="s">
+        <v>120</v>
+      </c>
       <c r="D78" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="E78" t="s">
-        <v>242</v>
+        <v>280</v>
       </c>
       <c r="F78" t="s">
-        <v>337</v>
+        <v>390</v>
       </c>
       <c r="G78" t="s">
-        <v>144</v>
+        <v>424</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79">
-        <v>1299680937</v>
+        <v>850512761</v>
       </c>
       <c r="B79" t="s">
         <v>84</v>
       </c>
       <c r="C79" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D79" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="E79" t="s">
-        <v>243</v>
+        <v>281</v>
       </c>
       <c r="F79" t="s">
-        <v>338</v>
+        <v>391</v>
       </c>
       <c r="G79" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80">
-        <v>779497488</v>
+        <v>452647583</v>
       </c>
       <c r="B80" t="s">
         <v>85</v>
       </c>
       <c r="C80" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="D80" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="E80" t="s">
-        <v>244</v>
+        <v>282</v>
       </c>
       <c r="F80" t="s">
-        <v>339</v>
+        <v>392</v>
       </c>
       <c r="G80" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81">
-        <v>850512761</v>
+        <v>5589926998</v>
       </c>
       <c r="B81" t="s">
         <v>86</v>
       </c>
       <c r="C81" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="D81" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="E81" t="s">
-        <v>245</v>
+        <v>283</v>
       </c>
       <c r="F81" t="s">
-        <v>340</v>
+        <v>393</v>
       </c>
       <c r="G81" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82">
-        <v>452647583</v>
+        <v>553113804</v>
       </c>
       <c r="B82" t="s">
         <v>87</v>
       </c>
       <c r="C82" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="D82" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="E82" t="s">
-        <v>246</v>
+        <v>284</v>
       </c>
       <c r="F82" t="s">
-        <v>341</v>
+        <v>394</v>
       </c>
       <c r="G82" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83">
-        <v>5589926998</v>
+        <v>541842024</v>
       </c>
       <c r="B83" t="s">
         <v>88</v>
       </c>
       <c r="C83" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="D83" t="s">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="E83" t="s">
-        <v>247</v>
+        <v>285</v>
       </c>
       <c r="F83" t="s">
-        <v>342</v>
+        <v>395</v>
       </c>
       <c r="G83" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84">
-        <v>553113804</v>
+        <v>5144589550</v>
       </c>
       <c r="B84" t="s">
         <v>89</v>
       </c>
       <c r="C84" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="D84" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="E84" t="s">
-        <v>248</v>
+        <v>286</v>
       </c>
       <c r="F84" t="s">
-        <v>343</v>
+        <v>396</v>
       </c>
       <c r="G84" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85">
-        <v>541842024</v>
+        <v>5955707709</v>
       </c>
       <c r="B85" t="s">
         <v>90</v>
       </c>
       <c r="C85" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="D85" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="E85" t="s">
-        <v>249</v>
+        <v>287</v>
       </c>
       <c r="F85" t="s">
-        <v>344</v>
+        <v>397</v>
       </c>
       <c r="G85" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86">
-        <v>5954496290</v>
+        <v>372702590</v>
       </c>
       <c r="B86" t="s">
         <v>91</v>
       </c>
       <c r="C86" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="D86" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E86" t="s">
-        <v>250</v>
+        <v>288</v>
       </c>
       <c r="F86" t="s">
-        <v>345</v>
+        <v>398</v>
       </c>
       <c r="G86" t="s">
-        <v>357</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87">
-        <v>5144589550</v>
+        <v>5583013175</v>
       </c>
       <c r="B87" t="s">
         <v>92</v>
       </c>
       <c r="C87" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="D87" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="E87" t="s">
-        <v>251</v>
+        <v>289</v>
       </c>
       <c r="F87" t="s">
-        <v>346</v>
+        <v>399</v>
       </c>
       <c r="G87" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88">
-        <v>5955707709</v>
+        <v>5954849896</v>
       </c>
       <c r="B88" t="s">
         <v>93</v>
       </c>
       <c r="C88" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="D88" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="E88" t="s">
-        <v>252</v>
+        <v>290</v>
       </c>
       <c r="F88" t="s">
-        <v>347</v>
+        <v>400</v>
       </c>
       <c r="G88" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89">
-        <v>372702590</v>
+        <v>1211422512</v>
       </c>
       <c r="B89" t="s">
         <v>94</v>
       </c>
       <c r="C89" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="D89" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="E89" t="s">
-        <v>253</v>
+        <v>291</v>
       </c>
       <c r="F89" t="s">
-        <v>348</v>
+        <v>401</v>
       </c>
       <c r="G89" t="s">
-        <v>141</v>
+        <v>424</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90">
-        <v>5583013175</v>
+        <v>768271026</v>
       </c>
       <c r="B90" t="s">
         <v>95</v>
       </c>
       <c r="C90" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="D90" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="E90" t="s">
-        <v>254</v>
+        <v>292</v>
       </c>
       <c r="F90" t="s">
-        <v>349</v>
+        <v>402</v>
       </c>
       <c r="G90" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91">
-        <v>5954849896</v>
+        <v>405879804</v>
       </c>
       <c r="B91" t="s">
         <v>96</v>
       </c>
       <c r="C91" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="D91" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="E91" t="s">
-        <v>255</v>
+        <v>293</v>
       </c>
       <c r="F91" t="s">
-        <v>350</v>
+        <v>403</v>
       </c>
       <c r="G91" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92">
-        <v>1211422512</v>
+        <v>2035636100</v>
       </c>
       <c r="B92" t="s">
         <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D92" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="E92" t="s">
-        <v>256</v>
+        <v>294</v>
       </c>
       <c r="F92" t="s">
-        <v>351</v>
+        <v>404</v>
       </c>
       <c r="G92" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93">
-        <v>768271026</v>
+        <v>5047490592</v>
       </c>
       <c r="B93" t="s">
         <v>98</v>
       </c>
       <c r="C93" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="D93" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="E93" t="s">
-        <v>257</v>
+        <v>295</v>
       </c>
       <c r="F93" t="s">
-        <v>352</v>
+        <v>405</v>
       </c>
       <c r="G93" t="s">
-        <v>357</v>
+        <v>425</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94">
-        <v>405879804</v>
+        <v>1359998197</v>
       </c>
       <c r="B94" t="s">
         <v>99</v>
       </c>
       <c r="C94" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="D94" t="s">
-        <v>158</v>
+        <v>188</v>
       </c>
       <c r="E94" t="s">
-        <v>258</v>
+        <v>296</v>
       </c>
       <c r="F94" t="s">
-        <v>353</v>
+        <v>406</v>
       </c>
       <c r="G94" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95">
-        <v>2035636100</v>
+        <v>1747806026</v>
       </c>
       <c r="B95" t="s">
         <v>100</v>
       </c>
       <c r="C95" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="D95" t="s">
-        <v>154</v>
+        <v>194</v>
       </c>
       <c r="E95" t="s">
-        <v>259</v>
+        <v>297</v>
       </c>
       <c r="F95" t="s">
-        <v>354</v>
+        <v>407</v>
       </c>
       <c r="G95" t="s">
-        <v>357</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96">
-        <v>5047490592</v>
+        <v>5541514013</v>
       </c>
       <c r="B96" t="s">
         <v>101</v>
       </c>
       <c r="C96" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="D96" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
       <c r="E96" t="s">
-        <v>260</v>
+        <v>298</v>
       </c>
       <c r="F96" t="s">
-        <v>355</v>
+        <v>407</v>
       </c>
       <c r="G96" t="s">
-        <v>358</v>
+        <v>174</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97">
-        <v>834865678</v>
+        <v>1294865508</v>
       </c>
       <c r="B97" t="s">
         <v>102</v>
       </c>
       <c r="C97" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="D97" t="s">
-        <v>129</v>
+        <v>196</v>
       </c>
       <c r="E97" t="s">
-        <v>261</v>
+        <v>299</v>
       </c>
       <c r="F97" t="s">
-        <v>356</v>
+        <v>408</v>
       </c>
       <c r="G97" t="s">
-        <v>358</v>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98">
+        <v>835862233</v>
+      </c>
+      <c r="B98" t="s">
+        <v>103</v>
+      </c>
+      <c r="C98" t="s">
+        <v>140</v>
+      </c>
+      <c r="D98" t="s">
+        <v>197</v>
+      </c>
+      <c r="E98" t="s">
+        <v>300</v>
+      </c>
+      <c r="F98" t="s">
+        <v>409</v>
+      </c>
+      <c r="G98" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99">
+        <v>791160917</v>
+      </c>
+      <c r="B99" t="s">
+        <v>104</v>
+      </c>
+      <c r="D99" t="s">
+        <v>198</v>
+      </c>
+      <c r="E99" t="s">
+        <v>301</v>
+      </c>
+      <c r="F99" t="s">
+        <v>410</v>
+      </c>
+      <c r="G99" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100">
+        <v>1499636883</v>
+      </c>
+      <c r="B100" t="s">
+        <v>105</v>
+      </c>
+      <c r="D100" t="s">
+        <v>199</v>
+      </c>
+      <c r="E100" t="s">
+        <v>302</v>
+      </c>
+      <c r="F100" t="s">
+        <v>411</v>
+      </c>
+      <c r="G100" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101">
+        <v>772365052</v>
+      </c>
+      <c r="B101" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" t="s">
+        <v>141</v>
+      </c>
+      <c r="D101" t="s">
+        <v>192</v>
+      </c>
+      <c r="E101" t="s">
+        <v>303</v>
+      </c>
+      <c r="F101" t="s">
+        <v>412</v>
+      </c>
+      <c r="G101" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102">
+        <v>1898052631</v>
+      </c>
+      <c r="B102" t="s">
+        <v>107</v>
+      </c>
+      <c r="C102" t="s">
+        <v>142</v>
+      </c>
+      <c r="D102" t="s">
+        <v>187</v>
+      </c>
+      <c r="E102" t="s">
+        <v>304</v>
+      </c>
+      <c r="F102" t="s">
+        <v>413</v>
+      </c>
+      <c r="G102" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103">
+        <v>834865678</v>
+      </c>
+      <c r="B103" t="s">
+        <v>108</v>
+      </c>
+      <c r="C103" t="s">
+        <v>143</v>
+      </c>
+      <c r="D103" t="s">
+        <v>158</v>
+      </c>
+      <c r="E103" t="s">
+        <v>305</v>
+      </c>
+      <c r="F103" t="s">
+        <v>414</v>
+      </c>
+      <c r="G103" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104">
+        <v>711488658</v>
+      </c>
+      <c r="B104" t="s">
+        <v>109</v>
+      </c>
+      <c r="C104" t="s">
+        <v>144</v>
+      </c>
+      <c r="D104" t="s">
+        <v>192</v>
+      </c>
+      <c r="E104" t="s">
+        <v>306</v>
+      </c>
+      <c r="F104" t="s">
+        <v>415</v>
+      </c>
+      <c r="G104" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105">
+        <v>1363091316</v>
+      </c>
+      <c r="B105" t="s">
+        <v>110</v>
+      </c>
+      <c r="C105" t="s">
+        <v>145</v>
+      </c>
+      <c r="D105" t="s">
+        <v>171</v>
+      </c>
+      <c r="E105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F105" t="s">
+        <v>416</v>
+      </c>
+      <c r="G105" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106">
+        <v>1374645480</v>
+      </c>
+      <c r="B106" t="s">
+        <v>111</v>
+      </c>
+      <c r="C106" t="s">
+        <v>146</v>
+      </c>
+      <c r="D106" t="s">
+        <v>200</v>
+      </c>
+      <c r="E106" t="s">
+        <v>308</v>
+      </c>
+      <c r="F106" t="s">
+        <v>417</v>
+      </c>
+      <c r="G106" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107">
+        <v>830225220</v>
+      </c>
+      <c r="B107" t="s">
+        <v>112</v>
+      </c>
+      <c r="C107" t="s">
+        <v>147</v>
+      </c>
+      <c r="D107" t="s">
+        <v>201</v>
+      </c>
+      <c r="E107" t="s">
+        <v>309</v>
+      </c>
+      <c r="F107" t="s">
+        <v>418</v>
+      </c>
+      <c r="G107" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108">
+        <v>5847315368</v>
+      </c>
+      <c r="B108" t="s">
+        <v>113</v>
+      </c>
+      <c r="C108" t="s">
+        <v>148</v>
+      </c>
+      <c r="D108" t="s">
+        <v>202</v>
+      </c>
+      <c r="E108" t="s">
+        <v>310</v>
+      </c>
+      <c r="F108" t="s">
+        <v>419</v>
+      </c>
+      <c r="G108" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109">
+        <v>5597035528</v>
+      </c>
+      <c r="B109" t="s">
+        <v>114</v>
+      </c>
+      <c r="C109" t="s">
+        <v>149</v>
+      </c>
+      <c r="D109" t="s">
+        <v>203</v>
+      </c>
+      <c r="E109" t="s">
+        <v>311</v>
+      </c>
+      <c r="F109" t="s">
+        <v>420</v>
+      </c>
+      <c r="G109" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110">
+        <v>646486428</v>
+      </c>
+      <c r="B110" t="s">
+        <v>115</v>
+      </c>
+      <c r="C110" t="s">
+        <v>150</v>
+      </c>
+      <c r="D110" t="s">
+        <v>199</v>
+      </c>
+      <c r="E110" t="s">
+        <v>312</v>
+      </c>
+      <c r="F110" t="s">
+        <v>421</v>
+      </c>
+      <c r="G110" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111">
+        <v>1730117172</v>
+      </c>
+      <c r="B111" t="s">
+        <v>116</v>
+      </c>
+      <c r="C111" t="s">
+        <v>151</v>
+      </c>
+      <c r="D111" t="s">
+        <v>174</v>
+      </c>
+      <c r="E111" t="s">
+        <v>313</v>
+      </c>
+      <c r="F111" t="s">
+        <v>422</v>
+      </c>
+      <c r="G111" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112">
+        <v>6594433913</v>
+      </c>
+      <c r="B112" t="s">
+        <v>117</v>
+      </c>
+      <c r="C112" t="s">
+        <v>152</v>
+      </c>
+      <c r="D112" t="s">
+        <v>192</v>
+      </c>
+      <c r="E112" t="s">
+        <v>314</v>
+      </c>
+      <c r="F112" t="s">
+        <v>423</v>
+      </c>
+      <c r="G112" t="s">
+        <v>424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>